<commit_message>
Tạo và cấu hình entity
</commit_message>
<xml_diff>
--- a/documents/designs/database.xlsx
+++ b/documents/designs/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A30070 - Tú Điền\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NET\NetCore\Project\CurriculumManager\CurriculumManager\documents\designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E32BE57-30B7-4DA0-A5A8-1E3BA18D37F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC20A2-97A2-417F-9C7C-4111467365C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BC8631EA-D656-42A1-8304-90F09B33E467}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BC8631EA-D656-42A1-8304-90F09B33E467}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -100,16 +99,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>220430</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>191855</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -124,8 +123,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1733550" y="438150"/>
-          <a:ext cx="1628775" cy="942975"/>
+          <a:off x="12221930" y="2669722"/>
+          <a:ext cx="1685925" cy="854528"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -184,16 +183,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>234037</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>129268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>195937</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>81641</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -208,8 +207,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4343400" y="428625"/>
-          <a:ext cx="1628775" cy="942975"/>
+          <a:off x="12235537" y="4129768"/>
+          <a:ext cx="1676400" cy="904873"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -417,7 +416,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>NumberCredit - Số</a:t>
+            <a:t>Unit - Số</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
@@ -507,16 +506,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>69388</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12246</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>59863</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -531,8 +530,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1790700" y="1590676"/>
-          <a:ext cx="1895475" cy="857250"/>
+          <a:off x="6682459" y="2107746"/>
+          <a:ext cx="1949904" cy="1130753"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -595,6 +594,26 @@
             </a:rPr>
             <a:t> nhóm kiến thức</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ParentId - Nhóm kiến thức cha</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>DisplayOrder - thử tự</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -613,14 +632,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>6808</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>156488</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -637,8 +656,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6572250" y="381000"/>
-          <a:ext cx="2047875" cy="1171575"/>
+          <a:off x="3680737" y="381000"/>
+          <a:ext cx="2109108" cy="1171575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -749,16 +768,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>63959</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>174172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>213638</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>78922</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -773,8 +792,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9391650" y="2324100"/>
-          <a:ext cx="3000375" cy="1238250"/>
+          <a:off x="11330673" y="364672"/>
+          <a:ext cx="3088822" cy="1238250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -855,7 +874,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Status - Trạng thái ( NotExist: 0 - Exist: 1)</a:t>
+            <a:t>InLibrary - Trạng thái ( NotExist: 0 - Exist: 1)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -881,14 +900,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>131993</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>27219</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -905,8 +924,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9391650" y="495300"/>
-          <a:ext cx="2990850" cy="942975"/>
+          <a:off x="6989993" y="495300"/>
+          <a:ext cx="3079297" cy="942975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1429,7 +1448,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Courses</a:t>
+            <a:t>SubjecId</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1466,70 +1485,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>147638</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59614087-8EC7-4A62-A687-316CA8845E10}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="3"/>
-          <a:endCxn id="3" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3362325" y="900113"/>
-          <a:ext cx="981075" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>156488</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>131993</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:to>
@@ -1549,8 +1512,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8620125" y="966788"/>
-          <a:ext cx="771525" cy="0"/>
+          <a:off x="5789845" y="966788"/>
+          <a:ext cx="1200148" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1578,16 +1541,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>27219</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>176213</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>63959</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>31297</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1599,14 +1562,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="7" idx="0"/>
-          <a:endCxn id="8" idx="2"/>
+          <a:stCxn id="7" idx="1"/>
+          <a:endCxn id="8" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="10887075" y="1438275"/>
-          <a:ext cx="4763" cy="885825"/>
+          <a:off x="10069290" y="966788"/>
+          <a:ext cx="1261383" cy="17009"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1858,16 +1821,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>159202</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>129270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>57148</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>81644</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1882,8 +1845,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6915150" y="3857625"/>
-          <a:ext cx="2047875" cy="1028700"/>
+          <a:off x="9221559" y="3939270"/>
+          <a:ext cx="2102303" cy="1285874"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1936,6 +1899,27 @@
             </a:rPr>
             <a:t>ID</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Name - Tên</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> chương trình học</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1983,8 +1967,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>214313</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>81648</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:to>
@@ -2004,12 +1988,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
-          <a:off x="1714500" y="381000"/>
-          <a:ext cx="5881688" cy="4205288"/>
+          <a:off x="1762125" y="381000"/>
+          <a:ext cx="2973166" cy="4205288"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -3887"/>
+            <a:gd name="adj1" fmla="val -7689"/>
             <a:gd name="adj2" fmla="val 105436"/>
           </a:avLst>
         </a:prstGeom>
@@ -2036,16 +2020,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>160562</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>137431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>65312</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2060,8 +2044,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6896100" y="2314575"/>
-          <a:ext cx="2047875" cy="742949"/>
+          <a:off x="9222919" y="2423431"/>
+          <a:ext cx="2109107" cy="869497"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2163,23 +2147,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>44899</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>44899</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Rectangle 47">
+        <xdr:cNvPr id="37" name="Rectangle 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7095E40A-92EE-463A-89F1-01F2B76C7FCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35066E00-BF82-4416-98C1-C7F5DBCE0F57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2187,8 +2171,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4219575" y="1562100"/>
-          <a:ext cx="2047875" cy="923925"/>
+          <a:off x="6657970" y="4000499"/>
+          <a:ext cx="1959429" cy="1156607"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2218,7 +2202,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>CurriculumDetails - Chi tiết chương trình học</a:t>
+            <a:t>CurriculumDetails - Chi tiết chương trình học </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -2242,6 +2226,16 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
+            <a:t>CurriculumId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t>KnowledgeGroupId</a:t>
           </a:r>
         </a:p>
@@ -2252,8 +2246,19 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>CurriculumId</a:t>
-          </a:r>
+            <a:t>Note</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> - Chú thích</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -2268,35 +2273,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>61913</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>49661</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>80963</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>64625</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+        <xdr:cNvPr id="45" name="Straight Arrow Connector 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8130917-2490-4F05-9320-BA5896B24451}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F84FB14-A4B3-4C79-B575-BC0C6DF3B07B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="46" idx="2"/>
-          <a:endCxn id="38" idx="0"/>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="37" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7920038" y="3057524"/>
-          <a:ext cx="19050" cy="800101"/>
+        <a:xfrm flipH="1">
+          <a:off x="7642447" y="3238499"/>
+          <a:ext cx="14964" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2324,40 +2329,38 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>83679</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>92523</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>129268</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+        <xdr:cNvPr id="49" name="Straight Arrow Connector 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{626AD63F-E34D-4F14-ABC2-A8AC84A5AE5F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DEF5DDC-A5E8-48D8-8644-7EC392D8D338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="3"/>
-          <a:endCxn id="38" idx="1"/>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5972175" y="900113"/>
-          <a:ext cx="942975" cy="3471862"/>
+          <a:off x="13064893" y="3524250"/>
+          <a:ext cx="8844" cy="605518"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -2382,140 +2385,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>44899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>6803</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="Rectangle 56">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D0AF89-BAB1-41DB-8763-50E72F5931EB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1790700" y="2695575"/>
-          <a:ext cx="1895475" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t> KnowledgeGroupDetails</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1">
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>KnowledgeGroupId</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>SubjectId</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="0">
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>159202</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10207</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="Straight Arrow Connector 58">
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DC9E4C8-C57C-4115-941B-3FDAD9AA092D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBFF2C4A-D780-4A31-AD8F-58EA95C68FEA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="5" idx="3"/>
-          <a:endCxn id="48" idx="1"/>
+          <a:stCxn id="38" idx="1"/>
+          <a:endCxn id="37" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3686175" y="2019301"/>
-          <a:ext cx="533400" cy="4762"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8617399" y="4578803"/>
+          <a:ext cx="604160" cy="3404"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2543,40 +2441,38 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>57148</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>80963</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>234037</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10207</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
+        <xdr:cNvPr id="60" name="Straight Arrow Connector 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DCCF82A-A549-498A-8B0B-78E651007599}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79B424B0-F450-4AD9-AD43-874578FD1F34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="38" idx="2"/>
-          <a:endCxn id="48" idx="2"/>
+          <a:stCxn id="3" idx="1"/>
+          <a:endCxn id="38" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1">
-          <a:off x="5391151" y="2338388"/>
-          <a:ext cx="2400300" cy="2695575"/>
+        <a:xfrm flipH="1">
+          <a:off x="11323862" y="4582205"/>
+          <a:ext cx="911675" cy="2"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -9524"/>
-          </a:avLst>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -2601,35 +2497,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119063</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>230640</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119063</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>235402</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>129270</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="64" name="Straight Arrow Connector 63">
+        <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B56A6C0-AFCA-4D07-94EE-60AC7106F2CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E54BC678-9A1D-4E75-8118-5A7A9B5CBE43}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="5" idx="2"/>
-          <a:endCxn id="57" idx="0"/>
+          <a:stCxn id="46" idx="2"/>
+          <a:endCxn id="38" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2738438" y="2447926"/>
-          <a:ext cx="0" cy="247649"/>
+        <a:xfrm flipH="1">
+          <a:off x="10272711" y="3292928"/>
+          <a:ext cx="4762" cy="646342"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2657,35 +2553,192 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119063</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119063</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>153762</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{182EBCA0-E54F-4EAD-B3DA-7902D05B37AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4327072" y="4014107"/>
+          <a:ext cx="1949904" cy="1130753"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectGroups</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>CurriculumDetailId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>153762</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>6803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>44899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>7484</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="Straight Arrow Connector 65">
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE37D371-72E1-4DAE-B4B4-B3F7EBF1DF0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD15C428-5292-44A5-A7E9-93E660FB639C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="0"/>
-          <a:endCxn id="57" idx="2"/>
+          <a:stCxn id="37" idx="1"/>
+          <a:endCxn id="30" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6276976" y="4578803"/>
+          <a:ext cx="380994" cy="681"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>7484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{732E4A8B-8457-403B-ACA3-DA5EA63ED70E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="30" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2738438" y="3552825"/>
-          <a:ext cx="0" cy="342901"/>
+          <a:off x="3864429" y="4579484"/>
+          <a:ext cx="462643" cy="6804"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3013,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31042CD-5974-448B-A340-A57F76A7793D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code màn hình SchoolYear, Faculty, Major, Subject
</commit_message>
<xml_diff>
--- a/documents/designs/database.xlsx
+++ b/documents/designs/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NET\NetCore\Project\CurriculumManager\CurriculumManager\documents\designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC20A2-97A2-417F-9C7C-4111467365C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05A582D-9F55-44EB-B29A-85AEC734F80C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BC8631EA-D656-42A1-8304-90F09B33E467}"/>
   </bookViews>
@@ -154,7 +154,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Facultys - Khoa</a:t>
+            <a:t>Faculties - Khoa</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -507,15 +507,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>69388</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>12246</xdr:rowOff>
+      <xdr:colOff>42173</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>189139</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>59863</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>32648</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -530,7 +530,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6682459" y="2107746"/>
+          <a:off x="6655244" y="2475139"/>
           <a:ext cx="1949904" cy="1130753"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -632,16 +632,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>6808</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>224897</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>156488</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>145521</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -656,8 +656,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3680737" y="381000"/>
-          <a:ext cx="2109108" cy="1171575"/>
+          <a:off x="2844272" y="370417"/>
+          <a:ext cx="3730624" cy="1402291"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -728,6 +728,16 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
+            <a:t>SchoolYearId - Mã năm học</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t>Goal - Mục tiêu học phần</a:t>
           </a:r>
         </a:p>
@@ -749,6 +759,23 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>Content - Nội dung chi tiết</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ApproveStatus - Trạng</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> thái (Approved: 0 - Reject: 1)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -770,14 +797,14 @@
     <xdr:from>
       <xdr:col>46</xdr:col>
       <xdr:colOff>63959</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>174172</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>94795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
       <xdr:colOff>213638</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>78922</xdr:rowOff>
+      <xdr:rowOff>184754</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -792,8 +819,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11330673" y="364672"/>
-          <a:ext cx="3088822" cy="1238250"/>
+          <a:off x="11017709" y="465212"/>
+          <a:ext cx="3007179" cy="1201209"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -900,16 +927,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>131993</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>12928</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>27219</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>146279</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>51856</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -924,8 +951,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6989993" y="495300"/>
-          <a:ext cx="3079297" cy="942975"/>
+          <a:off x="7156678" y="617007"/>
+          <a:ext cx="2990851" cy="916516"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1414,7 +1441,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>UserCourses </a:t>
+            <a:t>UserSubjects </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -1485,16 +1512,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>156488</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>145521</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:rowOff>145521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>131993</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>12928</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:rowOff>149223</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1512,8 +1539,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5789845" y="966788"/>
-          <a:ext cx="1200148" cy="0"/>
+          <a:off x="6574896" y="1071563"/>
+          <a:ext cx="581782" cy="3702"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1541,16 +1568,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>27219</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>146279</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:rowOff>139775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
       <xdr:colOff>63959</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>31297</xdr:rowOff>
+      <xdr:rowOff>149223</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1567,9 +1594,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="10069290" y="966788"/>
-          <a:ext cx="1261383" cy="17009"/>
+        <a:xfrm flipH="1">
+          <a:off x="10147529" y="1065817"/>
+          <a:ext cx="870180" cy="9448"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1823,14 +1850,14 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>159202</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>129270</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
       <xdr:colOff>57148</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>52918</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1845,8 +1872,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9221559" y="3939270"/>
-          <a:ext cx="2102303" cy="1285874"/>
+          <a:off x="8969827" y="3674688"/>
+          <a:ext cx="2041071" cy="1564063"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1946,6 +1973,16 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>SchoolYearId - Mã năm học</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ApproveStatus - Trạng thái (Approved: 0 - Reject: 1)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1964,13 +2001,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>81648</xdr:colOff>
+      <xdr:colOff>185209</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:rowOff>16935</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1988,13 +2025,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
-          <a:off x="1762125" y="381000"/>
-          <a:ext cx="2973166" cy="4205288"/>
+          <a:off x="1714500" y="370418"/>
+          <a:ext cx="2995084" cy="4091517"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -7689"/>
-            <a:gd name="adj2" fmla="val 105436"/>
+            <a:gd name="adj1" fmla="val -7633"/>
+            <a:gd name="adj2" fmla="val 105587"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2274,13 +2311,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>49661</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>37410</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>64625</xdr:colOff>
+      <xdr:colOff>44899</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
@@ -2299,9 +2336,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7642447" y="3238499"/>
-          <a:ext cx="14964" cy="762000"/>
+        <a:xfrm>
+          <a:off x="7630196" y="3605892"/>
+          <a:ext cx="7489" cy="394607"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2388,13 +2425,13 @@
       <xdr:col>35</xdr:col>
       <xdr:colOff>44899</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>6803</xdr:rowOff>
+      <xdr:rowOff>9449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>159202</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>10207</xdr:rowOff>
+      <xdr:rowOff>11720</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2412,8 +2449,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8617399" y="4578803"/>
-          <a:ext cx="604160" cy="3404"/>
+          <a:off x="8379274" y="4454449"/>
+          <a:ext cx="590553" cy="2271"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2444,13 +2481,13 @@
       <xdr:col>46</xdr:col>
       <xdr:colOff>57148</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>10205</xdr:rowOff>
+      <xdr:rowOff>11720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>234037</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>10207</xdr:rowOff>
+      <xdr:rowOff>12851</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2467,9 +2504,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11323862" y="4582205"/>
-          <a:ext cx="911675" cy="2"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11010898" y="4456720"/>
+          <a:ext cx="891264" cy="1131"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2498,15 +2535,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>230640</xdr:colOff>
+      <xdr:colOff>227238</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>54428</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>235402</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>129270</xdr:rowOff>
+      <xdr:colOff>232000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155730</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2524,8 +2561,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10272711" y="3292928"/>
-          <a:ext cx="4762" cy="646342"/>
+          <a:off x="9990363" y="3202970"/>
+          <a:ext cx="4762" cy="471718"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2742,6 +2779,287 @@
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F895972-28C6-4F70-91B9-5354C3D81B0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13566321" y="6068785"/>
+          <a:ext cx="2102304" cy="884464"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Genres - Bộ môn </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> - Tên bộ môn</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>FacultyId - Mã ngành</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>191855</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FEF6CA8-B8E6-4315-A6BF-EE8BACF408A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="33" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13907855" y="3096986"/>
+          <a:ext cx="709618" cy="2971799"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1361</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28CADEC3-C874-4EB7-9EF4-EC535AC0B246}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="2"/>
+          <a:endCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10177122" y="2655774"/>
+          <a:ext cx="142876" cy="8737826"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 688568"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>185210</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>232001</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>137431</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54BFF9C3-2EEA-4A99-A4A5-D27FA109C94F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="0"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="7058744" y="-576451"/>
+          <a:ext cx="587223" cy="5285541"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -3066,8 +3384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31042CD-5974-448B-A340-A57F76A7793D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AV30" sqref="AV30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code xong màn hình quản lý giáo viên
</commit_message>
<xml_diff>
--- a/documents/designs/database.xlsx
+++ b/documents/designs/database.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NET\NetCore\Project\CurriculumManager\CurriculumManager\documents\designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722860D0-4548-43CD-8EBA-01D3C73BAC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D67D31F-2953-4BC4-ACA0-6EEE52071703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BC8631EA-D656-42A1-8304-90F09B33E467}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{BC8631EA-D656-42A1-8304-90F09B33E467}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3075,6 +3077,945 @@
           <a:avLst>
             <a:gd name="adj1" fmla="val -17613"/>
           </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>572973</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>175244</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>57140</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>155632</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC285FC0-7118-4354-8ED4-034CF2057829}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17032173" y="2080244"/>
+          <a:ext cx="1922567" cy="932888"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Majors</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> - Ngành học</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Name - Tên</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> ngành (string)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>FacultyId (int)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>131939</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>353503</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28284</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A661AA-1C5A-4CC6-9064-B6CF0D5D1E61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="1846439"/>
+          <a:ext cx="2791903" cy="1420345"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Subjects</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> - Học phần </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectCode - Mã</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> học phần (string)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Name - Tên</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> học phần (string)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Unit - Số</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> tín chỉ (int)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Condition - Điều</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> kiện tiên quyết (string)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>HoursStudy - Số</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> giờ (string)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Coefficient - Hệ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> số (double)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>237997</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>259770</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>138115</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{635C3F17-8E0D-4C0B-BB0C-5555F4F1D03F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13649197" y="1714500"/>
+          <a:ext cx="2460173" cy="1662115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Curriculums</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> - Chương trình học</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Name - Tên</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> chương trình học (string)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>MajorId</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> - Mã ngành học (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SchoolYearId - Mã năm học (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ApproveStatus - Trạng thái (Approved: 0 - Reject: 1) (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>TuitionUnit - Đơn vị học phí</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>348873</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>237997</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66256</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{465F31B6-FFF5-4E5B-BC3D-EF37CA1A5CB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="7" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12540873" y="2540203"/>
+          <a:ext cx="1108324" cy="2553"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>259770</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66256</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>572973</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>67387</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D88C7C-4325-436A-AB14-F395B4675177}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="1"/>
+          <a:endCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="16109370" y="2542756"/>
+          <a:ext cx="922803" cy="1131"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>282197</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>49423</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>348873</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>77982</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39A312E4-35DF-48BF-9693-CABD6EC03AC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10645397" y="1954423"/>
+          <a:ext cx="1895476" cy="1171559"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectGroups</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Name (string)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Note (string)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>CurriculumId (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ParentId (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133881</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>48602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200557</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>77241</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90AA4CE5-0F1F-4899-9263-7D74AD7213AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7449081" y="2144102"/>
+          <a:ext cx="1895476" cy="790639"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectGroupDetail</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ID (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectGroupId (int)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>SubjectId (int)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>353503</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>62922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133881</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>77310</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC0877A-AE09-482D-BFEB-0C6AACCB6E18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5839903" y="2539422"/>
+          <a:ext cx="1609178" cy="14388"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200557</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>62922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>282197</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63703</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1028E1B0-FE37-4F24-91BB-7E6E4EE2B8E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="1"/>
+          <a:endCxn id="8" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9292602" y="2475097"/>
+          <a:ext cx="1293913" cy="781"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -3399,8 +4340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31042CD-5974-448B-A340-A57F76A7793D}">
   <dimension ref="I12:BW52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="45" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="CL21" sqref="CL21"/>
+    <sheetView topLeftCell="E14" zoomScale="68" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="BH30" activeCellId="2" sqref="BI35 BJ30 BH30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,4 +4490,22 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153E47D3-D7DD-4E99-8A1E-5CEDB7639BE4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="AC23" sqref="AC23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>